<commit_message>
updated chlorophyll data with data from station 25 provided by Jeanette Gann
</commit_message>
<xml_diff>
--- a/original_data/IYS-22 chlorophyll QC.xlsx
+++ b/original_data/IYS-22 chlorophyll QC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeane\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeane\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84947A3-C172-4649-8327-9F7609D0DC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CB39E5-FC95-4A07-8AC0-AEA80752BC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="122">
   <si>
     <t>Conc.</t>
   </si>
@@ -405,19 +405,30 @@
   <si>
     <t>b</t>
   </si>
+  <si>
+    <t>shimada</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
@@ -432,6 +443,17 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -509,36 +531,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -546,15 +569,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{FADA3CCE-BD6B-41C3-B85B-2A64F429F26A}"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -571,22 +614,22 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
+      <numFmt numFmtId="166" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000"/>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="168" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000000"/>
+      <numFmt numFmtId="169" formatCode="0.0000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.00000000"/>
+      <numFmt numFmtId="170" formatCode="0.00000000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4086,40 +4129,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y140"/>
+  <dimension ref="A1:Y148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B104" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I135" sqref="I135"/>
+      <selection pane="bottomRight" activeCell="S142" sqref="S142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="10" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.265625" style="2" customWidth="1"/>
-    <col min="12" max="13" width="9.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1328125" style="2"/>
-    <col min="17" max="17" width="14.3984375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.0546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.0546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.71875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.71875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.27734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.27734375" style="2" customWidth="1"/>
+    <col min="12" max="13" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.38671875" style="2" customWidth="1"/>
     <col min="18" max="18" width="9" style="2" customWidth="1"/>
-    <col min="19" max="19" width="10.73046875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="10.86328125" style="10" customWidth="1"/>
-    <col min="21" max="25" width="13.73046875" style="9" customWidth="1"/>
-    <col min="26" max="16384" width="9.1328125" style="2"/>
+    <col min="19" max="19" width="10.71875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="10.88671875" style="10" customWidth="1"/>
+    <col min="21" max="25" width="13.71875" style="9" customWidth="1"/>
+    <col min="26" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.5">
       <c r="P1" s="11" t="s">
         <v>46</v>
       </c>
@@ -4133,7 +4176,7 @@
         <v>0.26500000000000001</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
@@ -4210,7 +4253,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4286,7 +4329,7 @@
         <v>0.93236918367346899</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4362,7 +4405,7 @@
         <v>0.84223133781307324</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4442,7 +4485,7 @@
         <v>0.6409076205287717</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4520,7 +4563,7 @@
         <v>0.82179629005059018</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4596,7 +4639,7 @@
         <v>0.93150885072655221</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>1</v>
       </c>
@@ -4672,7 +4715,7 @@
         <v>3.1181704899777252</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>1</v>
       </c>
@@ -4748,7 +4791,7 @@
         <v>26.714911764705793</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>1</v>
       </c>
@@ -4824,7 +4867,7 @@
         <v>1.2903130645572847</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4900,7 +4943,7 @@
         <v>1.0507854368932033</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>1</v>
       </c>
@@ -4976,7 +5019,7 @@
         <v>0.7920752895752895</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>1</v>
       </c>
@@ -5056,7 +5099,7 @@
         <v>0.62835699658703015</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>1</v>
       </c>
@@ -5134,7 +5177,7 @@
         <v>0.79972586989409966</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>1</v>
       </c>
@@ -5210,7 +5253,7 @@
         <v>7.8371136363636467</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>1</v>
       </c>
@@ -5286,7 +5329,7 @@
         <v>10.422826086956519</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>1</v>
       </c>
@@ -5362,7 +5405,7 @@
         <v>3.2101739946380676</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>1</v>
       </c>
@@ -5438,7 +5481,7 @@
         <v>1.3833968864917867</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>1</v>
       </c>
@@ -5516,7 +5559,7 @@
         <v>0.91622840690978902</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>1</v>
       </c>
@@ -5596,7 +5639,7 @@
         <v>0.48613352668213494</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>1</v>
       </c>
@@ -5672,7 +5715,7 @@
         <v>1.1120861337683525</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>1</v>
       </c>
@@ -5748,7 +5791,7 @@
         <v>5.7223331521739134</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>1</v>
       </c>
@@ -5824,7 +5867,7 @@
         <v>9.7133416666666665</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>1</v>
       </c>
@@ -5900,7 +5943,7 @@
         <v>0.74560765349032843</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>1</v>
       </c>
@@ -5976,7 +6019,7 @@
         <v>0.81544865107913644</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>1</v>
       </c>
@@ -6052,7 +6095,7 @@
         <v>1.1705126923076925</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>1</v>
       </c>
@@ -6128,7 +6171,7 @@
         <v>0.78226288951841338</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>1</v>
       </c>
@@ -6204,7 +6247,7 @@
         <v>6.2300250248262223</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>1</v>
       </c>
@@ -6284,7 +6327,7 @@
         <v>9.1845285714285829</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>1</v>
       </c>
@@ -6362,7 +6405,7 @@
         <v>17.215599999999963</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>1</v>
       </c>
@@ -6438,7 +6481,7 @@
         <v>0.61666585677749342</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>1</v>
       </c>
@@ -6514,7 +6557,7 @@
         <v>1.1841059647302905</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>1</v>
       </c>
@@ -6590,7 +6633,7 @@
         <v>1.4539544203282158</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>1</v>
       </c>
@@ -6666,7 +6709,7 @@
         <v>7.8908000000000094</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>1</v>
       </c>
@@ -6744,7 +6787,7 @@
         <v>5.4141714968152845</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>1</v>
       </c>
@@ -6824,7 +6867,7 @@
         <v>4.3047368217054256</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>1</v>
       </c>
@@ -6900,7 +6943,7 @@
         <v>3.4088880299251865</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>1</v>
       </c>
@@ -6976,7 +7019,7 @@
         <v>1.6075478844169235</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>1</v>
       </c>
@@ -7052,7 +7095,7 @@
         <v>1.2296717482517476</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>1</v>
       </c>
@@ -7128,7 +7171,7 @@
         <v>1.1362557377049183</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>1</v>
       </c>
@@ -7204,7 +7247,7 @@
         <v>7.3874131799163152</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>1</v>
       </c>
@@ -7280,7 +7323,7 @@
         <v>6.6266560165975052</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>2</v>
       </c>
@@ -7358,7 +7401,7 @@
         <v>0.27084245901639342</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>2</v>
       </c>
@@ -7438,7 +7481,7 @@
         <v>0.21613891465677162</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>2</v>
       </c>
@@ -7514,7 +7557,7 @@
         <v>0.24429157105030924</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>2</v>
       </c>
@@ -7590,7 +7633,7 @@
         <v>0.15876517189835579</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>2</v>
       </c>
@@ -7666,7 +7709,7 @@
         <v>3.9842067901234577</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>2</v>
       </c>
@@ -7742,7 +7785,7 @@
         <v>0.67701515789473654</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>2</v>
       </c>
@@ -7820,7 +7863,7 @@
         <v>0.25691801980197998</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>2</v>
       </c>
@@ -7900,7 +7943,7 @@
         <v>0.30227105527638171</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>2</v>
       </c>
@@ -7976,7 +8019,7 @@
         <v>3.5003905861456484</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>2</v>
       </c>
@@ -8052,7 +8095,7 @@
         <v>0.17430113636363634</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>2</v>
       </c>
@@ -8132,7 +8175,7 @@
         <v>0.17221949541284423</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>2</v>
       </c>
@@ -8210,7 +8253,7 @@
         <v>0.14751566030385649</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A55">
         <v>2</v>
       </c>
@@ -8286,7 +8329,7 @@
         <v>0.23490137825421098</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A56">
         <v>2</v>
       </c>
@@ -8362,7 +8405,7 @@
         <v>0.37901433333333334</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A57">
         <v>2</v>
       </c>
@@ -8438,7 +8481,7 @@
         <v>1.290001523260601</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A58">
         <v>2</v>
       </c>
@@ -8514,7 +8557,7 @@
         <v>4.6476602352941185</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A59">
         <v>2</v>
       </c>
@@ -8594,7 +8637,7 @@
         <v>9.7899105545617204E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A60">
         <v>2</v>
       </c>
@@ -8672,7 +8715,7 @@
         <v>0.22513298429319351</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A61">
         <v>2</v>
       </c>
@@ -8748,7 +8791,7 @@
         <v>0.24660331632653038</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>2</v>
       </c>
@@ -8824,7 +8867,7 @@
         <v>0.16669728301886769</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A63">
         <v>2</v>
       </c>
@@ -8900,7 +8943,7 @@
         <v>0.41371456729288525</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A64">
         <v>2</v>
       </c>
@@ -8976,7 +9019,7 @@
         <v>0.53027450450450453</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A65">
         <v>2</v>
       </c>
@@ -9052,7 +9095,7 @@
         <v>3.2799365617433427</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A66">
         <v>2</v>
       </c>
@@ -9128,7 +9171,7 @@
         <v>0.20184894613583096</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A67">
         <v>2</v>
       </c>
@@ -9204,7 +9247,7 @@
         <v>0.30837506516073027</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A68">
         <v>2</v>
       </c>
@@ -9280,7 +9323,7 @@
         <v>0.23837211055276342</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A69">
         <v>2</v>
       </c>
@@ -9356,7 +9399,7 @@
         <v>0.85902498279421824</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A70">
         <v>2</v>
       </c>
@@ -9432,7 +9475,7 @@
         <v>1.4514214527845049</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A71">
         <v>2</v>
       </c>
@@ -9512,7 +9555,7 @@
         <v>5.4732520833333265</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A72">
         <v>2</v>
       </c>
@@ -9590,7 +9633,7 @@
         <v>7.6164069444444422</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A73">
         <v>2</v>
       </c>
@@ -9666,7 +9709,7 @@
         <v>0.53100159474671715</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A74">
         <v>2</v>
       </c>
@@ -9742,7 +9785,7 @@
         <v>0.46428219315895347</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A75">
         <v>2</v>
       </c>
@@ -9818,7 +9861,7 @@
         <v>0.55618121212121185</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A76">
         <v>2</v>
       </c>
@@ -9894,7 +9937,7 @@
         <v>5.3531681818181811</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A77">
         <v>2</v>
       </c>
@@ -9972,7 +10015,7 @@
         <v>0.81937062500000013</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A78">
         <v>2</v>
       </c>
@@ -10052,7 +10095,7 @@
         <v>0.8247493246623312</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A79">
         <v>2</v>
       </c>
@@ -10128,7 +10171,7 @@
         <v>0.47527919010123731</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A80">
         <v>2</v>
       </c>
@@ -10204,7 +10247,7 @@
         <v>0.33265587958607723</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A81">
         <v>2</v>
       </c>
@@ -10280,7 +10323,7 @@
         <v>0.41393818181818154</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A82">
         <v>2</v>
       </c>
@@ -10356,7 +10399,7 @@
         <v>0.42694493975903625</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A83">
         <v>3</v>
       </c>
@@ -10434,7 +10477,7 @@
         <v>0.46315782312925124</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A84">
         <v>3</v>
       </c>
@@ -10514,7 +10557,7 @@
         <v>0.39245975049244902</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A85">
         <v>3</v>
       </c>
@@ -10590,7 +10633,7 @@
         <v>6.4860407407407363</v>
       </c>
     </row>
-    <row r="86" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A86">
         <v>3</v>
       </c>
@@ -10666,7 +10709,7 @@
         <v>1.661019280205656</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A87">
         <v>3</v>
       </c>
@@ -10744,7 +10787,7 @@
         <v>0.56794279999999997</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A88">
         <v>3</v>
       </c>
@@ -10824,7 +10867,7 @@
         <v>0.65099610027855126</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A89">
         <v>3</v>
       </c>
@@ -10900,7 +10943,7 @@
         <v>0.440355813953488</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A90">
         <v>3</v>
       </c>
@@ -10976,7 +11019,7 @@
         <v>0.40268432203389798</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A91">
         <v>3</v>
       </c>
@@ -11052,7 +11095,7 @@
         <v>0.62706911196911175</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A92">
         <v>3</v>
       </c>
@@ -11128,7 +11171,7 @@
         <v>0.89671136131013351</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A93">
         <v>3</v>
       </c>
@@ -11204,7 +11247,7 @@
         <v>7.0396438423645336</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A94">
         <v>3</v>
       </c>
@@ -11280,7 +11323,7 @@
         <v>0.30051606029106009</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A95">
         <v>3</v>
       </c>
@@ -11356,7 +11399,7 @@
         <v>0.30177374556512937</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A96">
         <v>3</v>
       </c>
@@ -11432,7 +11475,7 @@
         <v>0.23622905811623277</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A97">
         <v>3</v>
       </c>
@@ -11508,7 +11551,7 @@
         <v>0.25215931677018621</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A98">
         <v>3</v>
       </c>
@@ -11584,7 +11627,7 @@
         <v>1.2204625092250923</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A99">
         <v>3</v>
       </c>
@@ -11664,7 +11707,7 @@
         <v>6.0182912280701721</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A100">
         <v>3</v>
       </c>
@@ -11742,7 +11785,7 @@
         <v>7.5523901315789388</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A101">
         <v>3</v>
       </c>
@@ -11818,7 +11861,7 @@
         <v>0.32560689655172392</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A102">
         <v>3</v>
       </c>
@@ -11898,7 +11941,7 @@
         <v>0.30380350467289696</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A103">
         <v>3</v>
       </c>
@@ -11976,7 +12019,7 @@
         <v>0.29346203115983838</v>
       </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A104">
         <v>3</v>
       </c>
@@ -12052,7 +12095,7 @@
         <v>0.19436556179775263</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A105">
         <v>3</v>
       </c>
@@ -12128,7 +12171,7 @@
         <v>0.52428952324897016</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A106">
         <v>3</v>
       </c>
@@ -12204,7 +12247,7 @@
         <v>2.9292499999999975</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A107">
         <v>3</v>
       </c>
@@ -12280,7 +12323,7 @@
         <v>9.9260238095238122</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A108">
         <v>3</v>
       </c>
@@ -12356,7 +12399,7 @@
         <v>0.20374882468168448</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A109">
         <v>3</v>
       </c>
@@ -12432,7 +12475,7 @@
         <v>0.17629985961628447</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A110">
         <v>3</v>
       </c>
@@ -12510,7 +12553,7 @@
         <v>0.28517321428571446</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A111">
         <v>3</v>
       </c>
@@ -12590,7 +12633,7 @@
         <v>0.17880895813047698</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A112">
         <v>3</v>
       </c>
@@ -12666,7 +12709,7 @@
         <v>0.56644090214067278</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A113">
         <v>3</v>
       </c>
@@ -12742,7 +12785,7 @@
         <v>2.9296089193825052</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A114">
         <v>3</v>
       </c>
@@ -12818,7 +12861,7 @@
         <v>4.052535504885995</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A115">
         <v>3</v>
       </c>
@@ -12898,7 +12941,7 @@
         <v>0.16312531311799594</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A116">
         <v>3</v>
       </c>
@@ -12974,7 +13017,7 @@
         <v>1.8936409302325574</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A117">
         <v>3</v>
       </c>
@@ -13050,7 +13093,7 @@
         <v>0.92755751295336719</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A118">
         <v>3</v>
       </c>
@@ -13126,7 +13169,7 @@
         <v>0.79102801556420199</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A119">
         <v>3</v>
       </c>
@@ -13202,7 +13245,7 @@
         <v>0.27664077163712181</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A120">
         <v>3</v>
       </c>
@@ -13280,7 +13323,7 @@
         <v>0.12104993581514754</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A121">
         <v>3</v>
       </c>
@@ -13356,7 +13399,7 @@
         <v>9.2990310077519414E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A122">
         <v>3</v>
       </c>
@@ -13432,7 +13475,7 @@
         <v>7.5798478571428527</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A123">
         <v>4</v>
       </c>
@@ -13510,7 +13553,7 @@
         <v>2.2586609116022092</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A124">
         <v>4</v>
       </c>
@@ -13590,7 +13633,7 @@
         <v>1.5458422535211249</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A125">
         <v>4</v>
       </c>
@@ -13666,7 +13709,7 @@
         <v>0.43996270491803258</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A126">
         <v>4</v>
       </c>
@@ -13742,7 +13785,7 @@
         <v>0.20848481375358172</v>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A127">
         <v>4</v>
       </c>
@@ -13818,7 +13861,7 @@
         <v>0.26533681012658228</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A128">
         <v>4</v>
       </c>
@@ -13894,7 +13937,7 @@
         <v>0.18461292246520872</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A129">
         <v>4</v>
       </c>
@@ -13970,7 +14013,7 @@
         <v>11.73453781094528</v>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A130">
         <v>4</v>
       </c>
@@ -14050,7 +14093,7 @@
         <v>1.0831346964064434</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A131">
         <v>4</v>
       </c>
@@ -14128,7 +14171,7 @@
         <v>1.7185170320404721</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A132">
         <v>4</v>
       </c>
@@ -14204,7 +14247,7 @@
         <v>0.75007020408163272</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A133">
         <v>4</v>
       </c>
@@ -14280,7 +14323,7 @@
         <v>0.28780526315789456</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A134">
         <v>4</v>
       </c>
@@ -14356,7 +14399,7 @@
         <v>0.19557456978967494</v>
       </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A135">
         <v>4</v>
       </c>
@@ -14432,7 +14475,7 @@
         <v>0.17192843403205926</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A136">
         <v>4</v>
       </c>
@@ -14508,7 +14551,7 @@
         <v>23.353465217391381</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A137">
         <v>4</v>
       </c>
@@ -14584,7 +14627,7 @@
         <v>7.4386335489086468</v>
       </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A138">
         <v>4</v>
       </c>
@@ -14660,7 +14703,7 @@
         <v>3.5358698529411758</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A139">
         <v>4</v>
       </c>
@@ -14736,81 +14779,316 @@
         <v>0.72904136043784229</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A140">
+    <row r="140" spans="1:25" s="25" customFormat="1" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A140" s="25">
         <v>4</v>
       </c>
-      <c r="B140" s="20">
+      <c r="B140" s="27">
         <v>44698</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="D140">
+      <c r="D140" s="25">
         <v>18</v>
       </c>
-      <c r="E140">
-        <v>1</v>
-      </c>
-      <c r="F140">
+      <c r="E140" s="25">
+        <v>1</v>
+      </c>
+      <c r="F140" s="25">
         <v>25</v>
       </c>
-      <c r="G140" t="s">
+      <c r="G140" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="H140"/>
-      <c r="I140"/>
-      <c r="J140"/>
-      <c r="K140">
+      <c r="K140" s="25">
         <v>18</v>
       </c>
-      <c r="L140">
+      <c r="L140" s="25">
         <v>29.98</v>
       </c>
-      <c r="M140" s="23">
+      <c r="M140" s="28">
         <v>18.309999999999999</v>
       </c>
-      <c r="N140">
+      <c r="N140" s="25">
         <v>110.2</v>
       </c>
-      <c r="O140" s="23">
+      <c r="O140" s="28">
         <v>67.209999999999994</v>
       </c>
-      <c r="P140">
-        <v>1</v>
-      </c>
-      <c r="Q140">
-        <v>5</v>
-      </c>
-      <c r="R140">
+      <c r="P140" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q140" s="25">
+        <v>5</v>
+      </c>
+      <c r="R140" s="25">
         <v>250</v>
       </c>
-      <c r="S140">
+      <c r="S140" s="25">
         <v>284</v>
       </c>
-      <c r="T140">
+      <c r="T140" s="25">
         <v>1.0452077289292201</v>
       </c>
-      <c r="U140" s="9">
+      <c r="U140" s="29">
         <f t="shared" si="10"/>
         <v>23.238014834818298</v>
       </c>
-      <c r="V140" s="9">
+      <c r="V140" s="29">
         <f t="shared" si="11"/>
         <v>0.40911997948623763</v>
       </c>
-      <c r="W140" s="9">
+      <c r="W140" s="29">
         <f t="shared" si="12"/>
         <v>14.941188937684315</v>
       </c>
-      <c r="X140" s="9">
+      <c r="X140" s="29">
         <f t="shared" si="13"/>
         <v>0.26304910101556889</v>
       </c>
-      <c r="Y140" s="9">
+      <c r="Y140" s="29">
         <f t="shared" si="14"/>
         <v>0.64296322400558203</v>
       </c>
+    </row>
+    <row r="141" spans="1:25" s="25" customFormat="1" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A141" s="34"/>
+      <c r="C141" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E141" s="34">
+        <v>25</v>
+      </c>
+      <c r="F141" s="34">
+        <v>5</v>
+      </c>
+      <c r="G141" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="L141" s="30"/>
+      <c r="M141" s="30"/>
+      <c r="P141" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q141" s="31">
+        <v>6</v>
+      </c>
+      <c r="S141" s="34">
+        <v>284</v>
+      </c>
+      <c r="V141" s="32">
+        <v>0.36157340415098388</v>
+      </c>
+      <c r="X141" s="32">
+        <v>0.14690479724545896</v>
+      </c>
+    </row>
+    <row r="142" spans="1:25" s="25" customFormat="1" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A142" s="34"/>
+      <c r="C142" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E142" s="34">
+        <v>25</v>
+      </c>
+      <c r="F142" s="34">
+        <v>25</v>
+      </c>
+      <c r="G142" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H142" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="L142" s="30"/>
+      <c r="M142" s="30"/>
+      <c r="P142" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q142" s="31">
+        <v>6</v>
+      </c>
+      <c r="S142" s="34">
+        <v>284</v>
+      </c>
+      <c r="V142" s="32">
+        <v>0.36622423356906408</v>
+      </c>
+      <c r="X142" s="32">
+        <v>0.12997276409164152</v>
+      </c>
+    </row>
+    <row r="143" spans="1:25" s="25" customFormat="1" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A143" s="34"/>
+      <c r="C143" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E143" s="34">
+        <v>25</v>
+      </c>
+      <c r="F143" s="35">
+        <v>25</v>
+      </c>
+      <c r="G143" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H143" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="L143" s="30"/>
+      <c r="M143" s="30"/>
+      <c r="P143" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q143" s="31">
+        <v>6</v>
+      </c>
+      <c r="S143" s="34">
+        <v>284</v>
+      </c>
+      <c r="V143" s="32">
+        <v>0.33407894703519997</v>
+      </c>
+      <c r="X143" s="32">
+        <v>0.13108754899738417</v>
+      </c>
+    </row>
+    <row r="144" spans="1:25" s="25" customFormat="1" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A144" s="34"/>
+      <c r="C144" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E144" s="34">
+        <v>25</v>
+      </c>
+      <c r="F144" s="34">
+        <v>50</v>
+      </c>
+      <c r="G144" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="L144" s="30"/>
+      <c r="M144" s="30"/>
+      <c r="P144" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q144" s="31">
+        <v>6</v>
+      </c>
+      <c r="S144" s="34">
+        <v>284</v>
+      </c>
+      <c r="V144" s="32">
+        <v>0.33813797078144436</v>
+      </c>
+      <c r="X144" s="32">
+        <v>0.16050993979988221</v>
+      </c>
+    </row>
+    <row r="145" spans="1:25" s="25" customFormat="1" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A145" s="34"/>
+      <c r="C145" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E145" s="34">
+        <v>25</v>
+      </c>
+      <c r="F145" s="34">
+        <v>75</v>
+      </c>
+      <c r="G145" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="L145" s="30"/>
+      <c r="M145" s="30"/>
+      <c r="P145" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q145" s="31">
+        <v>6</v>
+      </c>
+      <c r="S145" s="34">
+        <v>284</v>
+      </c>
+      <c r="V145" s="32">
+        <v>0.31066157131192818</v>
+      </c>
+      <c r="X145" s="32">
+        <v>0.13296897824650264</v>
+      </c>
+    </row>
+    <row r="146" spans="1:25" s="25" customFormat="1" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A146" s="34"/>
+      <c r="C146" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E146" s="34">
+        <v>25</v>
+      </c>
+      <c r="F146" s="34">
+        <v>100</v>
+      </c>
+      <c r="G146" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="L146" s="30"/>
+      <c r="M146" s="30"/>
+      <c r="P146" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q146" s="31">
+        <v>6</v>
+      </c>
+      <c r="S146" s="34">
+        <v>284</v>
+      </c>
+      <c r="V146" s="32">
+        <v>0.11418918017395903</v>
+      </c>
+      <c r="X146" s="32">
+        <v>7.6211437352612432E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:25" s="25" customFormat="1" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A147" s="34"/>
+      <c r="C147" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E147" s="34">
+        <v>25</v>
+      </c>
+      <c r="F147" s="34">
+        <v>150</v>
+      </c>
+      <c r="G147" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="L147" s="30"/>
+      <c r="M147" s="30"/>
+      <c r="P147" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q147" s="31">
+        <v>6</v>
+      </c>
+      <c r="S147" s="34">
+        <v>284</v>
+      </c>
+      <c r="V147" s="32">
+        <v>1.0786333869227898E-2</v>
+      </c>
+      <c r="X147" s="32">
+        <v>2.2949091725018893E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:25" s="25" customFormat="1" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="T148" s="33"/>
+      <c r="U148" s="29"/>
+      <c r="V148" s="29"/>
+      <c r="W148" s="29"/>
+      <c r="X148" s="29"/>
+      <c r="Y148" s="29"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Y57">
@@ -14830,31 +15108,31 @@
       <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="10" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.27734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.38671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.27734375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.265625" style="2" customWidth="1"/>
-    <col min="12" max="13" width="9.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1328125" style="2"/>
-    <col min="17" max="17" width="14.3984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.71875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.71875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.27734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.27734375" style="2" customWidth="1"/>
+    <col min="12" max="13" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.38671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="2"/>
+    <col min="17" max="17" width="14.38671875" style="2" customWidth="1"/>
     <col min="18" max="18" width="9" style="2" customWidth="1"/>
-    <col min="19" max="19" width="10.73046875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="10.86328125" style="10" customWidth="1"/>
-    <col min="21" max="25" width="13.73046875" style="9" customWidth="1"/>
-    <col min="26" max="16384" width="9.1328125" style="2"/>
+    <col min="19" max="19" width="10.71875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="10.88671875" style="10" customWidth="1"/>
+    <col min="21" max="25" width="13.71875" style="9" customWidth="1"/>
+    <col min="26" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.5">
       <c r="P1" s="11" t="s">
         <v>46</v>
       </c>
@@ -14868,7 +15146,7 @@
         <v>0.26500000000000001</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
@@ -14945,7 +15223,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -15023,7 +15301,7 @@
         <v>0.6409076205287717</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -15099,7 +15377,7 @@
         <v>0.82179629005059018</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -15177,7 +15455,7 @@
         <v>0.62835699658703015</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>1</v>
       </c>
@@ -15253,7 +15531,7 @@
         <v>0.79972586989409966</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>1</v>
       </c>
@@ -15329,7 +15607,7 @@
         <v>0.91622840690978902</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>1</v>
       </c>
@@ -15407,7 +15685,7 @@
         <v>0.48613352668213494</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>1</v>
       </c>
@@ -15485,7 +15763,7 @@
         <v>9.1845285714285829</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>1</v>
       </c>
@@ -15561,7 +15839,7 @@
         <v>17.215599999999963</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>1</v>
       </c>
@@ -15637,7 +15915,7 @@
         <v>5.4141714968152845</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>1</v>
       </c>
@@ -15715,7 +15993,7 @@
         <v>4.3047368217054256</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>2</v>
       </c>
@@ -15791,7 +16069,7 @@
         <v>0.27084245901639342</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>2</v>
       </c>
@@ -15869,7 +16147,7 @@
         <v>0.21613891465677162</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>2</v>
       </c>
@@ -15945,7 +16223,7 @@
         <v>0.25691801980197998</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>2</v>
       </c>
@@ -16023,7 +16301,7 @@
         <v>0.30227105527638171</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>2</v>
       </c>
@@ -16101,7 +16379,7 @@
         <v>0.17221949541284423</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>2</v>
       </c>
@@ -16177,7 +16455,7 @@
         <v>0.14751566030385649</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>2</v>
       </c>
@@ -16255,7 +16533,7 @@
         <v>9.7899105545617204E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>2</v>
       </c>
@@ -16331,7 +16609,7 @@
         <v>0.22513298429319351</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>2</v>
       </c>
@@ -16409,7 +16687,7 @@
         <v>5.4732520833333265</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>2</v>
       </c>
@@ -16485,7 +16763,7 @@
         <v>7.6164069444444422</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>2</v>
       </c>
@@ -16561,7 +16839,7 @@
         <v>0.81937062500000013</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>2</v>
       </c>
@@ -16639,7 +16917,7 @@
         <v>0.8247493246623312</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>3</v>
       </c>
@@ -16710,7 +16988,7 @@
         <v>0.46315782312925124</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>3</v>
       </c>
@@ -16783,7 +17061,7 @@
         <v>0.39245975049244902</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>3</v>
       </c>
@@ -16854,7 +17132,7 @@
         <v>0.56794279999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>3</v>
       </c>
@@ -16927,7 +17205,7 @@
         <v>0.65099610027855126</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>3</v>
       </c>
@@ -17000,7 +17278,7 @@
         <v>6.0182912280701721</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>3</v>
       </c>
@@ -17071,7 +17349,7 @@
         <v>7.5523901315789388</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>3</v>
       </c>
@@ -17144,7 +17422,7 @@
         <v>0.30380350467289696</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>3</v>
       </c>
@@ -17215,7 +17493,7 @@
         <v>0.29346203115983838</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>3</v>
       </c>
@@ -17286,7 +17564,7 @@
         <v>0.28517321428571446</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>3</v>
       </c>
@@ -17359,7 +17637,7 @@
         <v>0.17880895813047698</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>3</v>
       </c>
@@ -17432,7 +17710,7 @@
         <v>0.16312531311799594</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>3</v>
       </c>
@@ -17503,7 +17781,7 @@
         <v>0.12104993581514754</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>4</v>
       </c>
@@ -17574,7 +17852,7 @@
         <v>2.2586609116022092</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>4</v>
       </c>
@@ -17647,7 +17925,7 @@
         <v>1.5458422535211249</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>4</v>
       </c>
@@ -17720,7 +17998,7 @@
         <v>1.0831346964064434</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>4</v>
       </c>
@@ -17791,7 +18069,7 @@
         <v>1.7185170320404721</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.5">
       <c r="B42" s="17" t="s">
         <v>54</v>
       </c>
@@ -17802,7 +18080,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.5">
       <c r="B43" s="18">
         <v>51</v>
       </c>
@@ -17813,7 +18091,7 @@
         <v>3.3586543588695582E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.5">
       <c r="B44" s="18">
         <v>47</v>
       </c>
@@ -17824,7 +18102,7 @@
         <v>0.14643733004672707</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.5">
       <c r="B45" s="18">
         <v>49</v>
       </c>
@@ -17835,7 +18113,7 @@
         <v>0.22906022727492706</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.5">
       <c r="B46" s="18">
         <v>45</v>
       </c>
@@ -17846,7 +18124,7 @@
         <v>7.3218665023363451E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.5">
       <c r="B47" s="18">
         <v>43</v>
       </c>
@@ -17857,7 +18135,7 @@
         <v>9.80727072790007E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.5">
       <c r="B48" s="18">
         <v>39</v>
       </c>
@@ -17868,7 +18146,7 @@
         <v>0.2207805942258064</v>
       </c>
     </row>
-    <row r="49" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B49" s="18">
         <v>41</v>
       </c>
@@ -17879,7 +18157,7 @@
         <v>1.0158616298744729E-2</v>
       </c>
     </row>
-    <row r="50" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B50" s="18">
         <v>37</v>
       </c>
@@ -17891,7 +18169,7 @@
       </c>
       <c r="E50" s="19"/>
     </row>
-    <row r="51" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B51" s="18">
         <v>35</v>
       </c>
@@ -17911,7 +18189,7 @@
       <c r="X51" s="2"/>
       <c r="Y51" s="2"/>
     </row>
-    <row r="52" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B52" s="18">
         <v>33</v>
       </c>
@@ -17931,7 +18209,7 @@
       <c r="X52" s="2"/>
       <c r="Y52" s="2"/>
     </row>
-    <row r="53" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B53" s="18">
         <v>31</v>
       </c>
@@ -17951,7 +18229,7 @@
       <c r="X53" s="2"/>
       <c r="Y53" s="2"/>
     </row>
-    <row r="54" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B54" s="18">
         <v>27</v>
       </c>
@@ -17971,7 +18249,7 @@
       <c r="X54" s="2"/>
       <c r="Y54" s="2"/>
     </row>
-    <row r="55" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B55" s="18">
         <v>29</v>
       </c>
@@ -17982,7 +18260,7 @@
         <v>2.1587967992942825E-2</v>
       </c>
     </row>
-    <row r="56" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B56" s="18">
         <v>23</v>
       </c>
@@ -17993,7 +18271,7 @@
         <v>1.2817855995809527E-3</v>
       </c>
     </row>
-    <row r="57" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B57" s="18">
         <v>21</v>
       </c>
@@ -18004,7 +18282,7 @@
         <v>1.4167103995360154E-2</v>
       </c>
     </row>
-    <row r="58" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B58" s="18">
         <v>19</v>
       </c>
@@ -18015,7 +18293,7 @@
         <v>0.21453043192986207</v>
       </c>
     </row>
-    <row r="59" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B59" s="18">
         <v>17</v>
       </c>
@@ -18026,7 +18304,7 @@
         <v>2.7659583990964843E-2</v>
       </c>
     </row>
-    <row r="60" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B60" s="18">
         <v>15</v>
       </c>
@@ -18037,7 +18315,7 @@
         <v>1.8169041216487092E-2</v>
       </c>
     </row>
-    <row r="61" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B61" s="18">
         <v>4</v>
       </c>
@@ -18048,7 +18326,7 @@
         <v>0.12301113831014117</v>
       </c>
     </row>
-    <row r="64" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B64" s="2" t="s">
         <v>54</v>
       </c>
@@ -18062,7 +18340,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B65" s="2">
         <v>51</v>
       </c>
@@ -18077,7 +18355,7 @@
         <v>5.7209286503760231</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B66" s="2">
         <v>47</v>
       </c>
@@ -18092,7 +18370,7 @@
         <v>20.019386792034663</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B67" s="2">
         <v>49</v>
       </c>
@@ -18107,7 +18385,7 @@
         <v>34.869618566104542</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B68" s="2">
         <v>45</v>
       </c>
@@ -18122,7 +18400,7 @@
         <v>47.430547168820546</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B69" s="2">
         <v>43</v>
       </c>
@@ -18137,7 +18415,7 @@
         <v>14.727188310019345</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B70" s="2">
         <v>39</v>
       </c>
@@ -18152,7 +18430,7 @@
         <v>11.566322662660298</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B71" s="2">
         <v>41</v>
       </c>
@@ -18167,7 +18445,7 @@
         <v>1.0580151339461603</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B72" s="2">
         <v>37</v>
       </c>
@@ -18182,7 +18460,7 @@
         <v>1.3369952644472789</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B73" s="2">
         <v>35</v>
       </c>
@@ -18197,7 +18475,7 @@
         <v>1.7490273739610207</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B74" s="2">
         <v>33</v>
       </c>
@@ -18212,7 +18490,7 @@
         <v>20.203050891044274</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B75" s="2">
         <v>31</v>
       </c>
@@ -18227,7 +18505,7 @@
         <v>12.891558047547377</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B76" s="2">
         <v>27</v>
       </c>
@@ -18242,7 +18520,7 @@
         <v>9.9382541277094649</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B77" s="2">
         <v>29</v>
       </c>
@@ -18257,7 +18535,7 @@
         <v>3.0827543593965312</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B78" s="2">
         <v>23</v>
       </c>
@@ -18272,7 +18550,7 @@
         <v>8.3189033080772194</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B79" s="2">
         <v>21</v>
       </c>
@@ -18287,7 +18565,7 @@
         <v>0.86207503076395786</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B80" s="2">
         <v>19</v>
       </c>
@@ -18302,7 +18580,7 @@
         <v>11.865960760808687</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B81" s="2">
         <v>17</v>
       </c>
@@ -18317,7 +18595,7 @@
         <v>1.8856180831646778</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B82" s="2">
         <v>15</v>
       </c>
@@ -18332,7 +18610,7 @@
         <v>22.225707906911353</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B83" s="2">
         <v>4</v>
       </c>
@@ -18361,32 +18639,32 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="10" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.38671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.27734375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.265625" style="2" customWidth="1"/>
-    <col min="12" max="13" width="9.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.3984375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="9.1328125" style="2"/>
-    <col min="18" max="18" width="14.3984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.71875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.71875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.27734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.27734375" style="2" customWidth="1"/>
+    <col min="12" max="13" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.38671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.38671875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="2"/>
+    <col min="18" max="18" width="14.38671875" style="2" customWidth="1"/>
     <col min="19" max="19" width="9" style="2" customWidth="1"/>
-    <col min="20" max="20" width="10.73046875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="10.86328125" style="10" customWidth="1"/>
-    <col min="22" max="26" width="13.73046875" style="9" customWidth="1"/>
-    <col min="27" max="16384" width="9.1328125" style="2"/>
+    <col min="20" max="20" width="10.71875" style="2" customWidth="1"/>
+    <col min="21" max="21" width="10.88671875" style="10" customWidth="1"/>
+    <col min="22" max="26" width="13.71875" style="9" customWidth="1"/>
+    <col min="27" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.5">
       <c r="Q1" s="11" t="s">
         <v>46</v>
       </c>
@@ -18400,7 +18678,7 @@
         <v>0.26500000000000001</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
@@ -18477,7 +18755,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -18565,7 +18843,7 @@
         <v>2.6694049928673333</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -18653,7 +18931,7 @@
         <v>1.7609146574614973</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -18741,7 +19019,7 @@
         <v>11.797408411214953</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -18829,7 +19107,7 @@
         <v>0.60180236813778265</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -18917,7 +19195,7 @@
         <v>1.0416372734761119</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -19005,7 +19283,7 @@
         <v>8.0668558441558478</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -19093,7 +19371,7 @@
         <v>3.5460875539568342</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -19181,7 +19459,7 @@
         <v>0.69359917355371892</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -19287,22 +19565,22 @@
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="17.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.38671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.71875" style="1" customWidth="1"/>
     <col min="5" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1328125" style="1"/>
-    <col min="8" max="8" width="12.73046875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.1328125" style="1"/>
-    <col min="11" max="11" width="12.86328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1328125" style="1" customWidth="1"/>
-    <col min="13" max="14" width="14.59765625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1328125" style="1"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="8" width="12.71875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="1"/>
+    <col min="11" max="11" width="12.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="14.609375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="34.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -19346,7 +19624,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -19394,7 +19672,7 @@
         <v>1.0068529678983578</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -19422,7 +19700,7 @@
         <v>152.9</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -19470,7 +19748,7 @@
         <v>1.030154185496019</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -19498,7 +19776,7 @@
         <v>147.5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -19515,7 +19793,7 @@
         <v>87.1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -19532,7 +19810,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -19549,7 +19827,7 @@
         <v>576.20000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -19566,7 +19844,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -19583,7 +19861,7 @@
         <v>-0.23300000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -19600,7 +19878,7 @@
         <v>0.157</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -19617,7 +19895,7 @@
         <v>557.9</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -19634,7 +19912,7 @@
         <v>84.46</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -19642,7 +19920,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>23.885000000000002</v>
       </c>
@@ -19650,15 +19928,15 @@
         <v>154.85</v>
       </c>
     </row>
-    <row r="17" spans="10:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="10:11" x14ac:dyDescent="0.55000000000000004">
       <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="10:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="10:11" x14ac:dyDescent="0.55000000000000004">
       <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="10:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.55000000000000004">
       <c r="J19"/>
       <c r="K19"/>
     </row>
@@ -19674,13 +19952,13 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.27734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.38671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="17" t="s">
         <v>54</v>
       </c>
@@ -19688,7 +19966,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="18" t="s">
         <v>58</v>
       </c>
@@ -19696,7 +19974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="18" t="s">
         <v>59</v>
       </c>
@@ -19704,7 +19982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="18" t="s">
         <v>60</v>
       </c>
@@ -19712,7 +19990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="18" t="s">
         <v>61</v>
       </c>
@@ -19720,7 +19998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="18" t="s">
         <v>62</v>
       </c>
@@ -19728,7 +20006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="18" t="s">
         <v>63</v>
       </c>
@@ -19736,7 +20014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="18" t="s">
         <v>64</v>
       </c>
@@ -19744,7 +20022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="18" t="s">
         <v>68</v>
       </c>
@@ -19752,7 +20030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
         <v>69</v>
       </c>
@@ -19760,7 +20038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="18" t="s">
         <v>72</v>
       </c>
@@ -19768,7 +20046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" s="18" t="s">
         <v>76</v>
       </c>
@@ -19776,7 +20054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" s="18" t="s">
         <v>81</v>
       </c>
@@ -19784,7 +20062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" s="18" t="s">
         <v>82</v>
       </c>
@@ -19792,7 +20070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" s="18" t="s">
         <v>85</v>
       </c>
@@ -19800,7 +20078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" s="18" t="s">
         <v>86</v>
       </c>
@@ -19808,7 +20086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="18" t="s">
         <v>88</v>
       </c>
@@ -19816,7 +20094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" s="18" t="s">
         <v>90</v>
       </c>
@@ -19824,7 +20102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" s="18" t="s">
         <v>93</v>
       </c>
@@ -19832,7 +20110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" s="18" t="s">
         <v>94</v>
       </c>
@@ -19840,7 +20118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" s="18" t="s">
         <v>95</v>
       </c>
@@ -19848,7 +20126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" s="18" t="s">
         <v>96</v>
       </c>
@@ -19856,7 +20134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" s="18" t="s">
         <v>97</v>
       </c>
@@ -19864,7 +20142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" s="18" t="s">
         <v>98</v>
       </c>
@@ -19872,7 +20150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" s="18" t="s">
         <v>99</v>
       </c>
@@ -19880,7 +20158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" s="18" t="s">
         <v>100</v>
       </c>
@@ -19888,7 +20166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" s="18" t="s">
         <v>103</v>
       </c>
@@ -19896,7 +20174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" s="18" t="s">
         <v>104</v>
       </c>
@@ -19904,7 +20182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29" s="18" t="s">
         <v>106</v>
       </c>
@@ -19912,7 +20190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" s="18" t="s">
         <v>108</v>
       </c>
@@ -19920,7 +20198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" s="18" t="s">
         <v>111</v>
       </c>
@@ -19928,7 +20206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" s="18" t="s">
         <v>112</v>
       </c>
@@ -19936,7 +20214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" s="18" t="s">
         <v>66</v>
       </c>
@@ -19944,7 +20222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" s="18" t="s">
         <v>67</v>
       </c>
@@ -19952,7 +20230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" s="18" t="s">
         <v>71</v>
       </c>
@@ -19960,7 +20238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" s="18" t="s">
         <v>75</v>
       </c>
@@ -19968,7 +20246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" s="18" t="s">
         <v>79</v>
       </c>
@@ -19976,7 +20254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" s="18" t="s">
         <v>80</v>
       </c>
@@ -19984,7 +20262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" s="18" t="s">
         <v>83</v>
       </c>
@@ -19992,7 +20270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40" s="18" t="s">
         <v>84</v>
       </c>
@@ -20000,7 +20278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41" s="18" t="s">
         <v>87</v>
       </c>
@@ -20008,7 +20286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42" s="18" t="s">
         <v>89</v>
       </c>
@@ -20016,7 +20294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" s="18" t="s">
         <v>92</v>
       </c>
@@ -20024,7 +20302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" s="18" t="s">
         <v>91</v>
       </c>
@@ -20032,7 +20310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" s="18" t="s">
         <v>101</v>
       </c>
@@ -20040,7 +20318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" s="18" t="s">
         <v>102</v>
       </c>
@@ -20048,7 +20326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" s="18" t="s">
         <v>105</v>
       </c>
@@ -20056,7 +20334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" s="18" t="s">
         <v>107</v>
       </c>
@@ -20064,7 +20342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" s="18" t="s">
         <v>110</v>
       </c>
@@ -20072,7 +20350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" s="18" t="s">
         <v>109</v>
       </c>
@@ -20080,7 +20358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51" s="18" t="s">
         <v>65</v>
       </c>
@@ -20088,7 +20366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A52" s="18" t="s">
         <v>70</v>
       </c>
@@ -20096,7 +20374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A53" s="18" t="s">
         <v>73</v>
       </c>
@@ -20104,7 +20382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A54" s="18" t="s">
         <v>74</v>
       </c>
@@ -20112,7 +20390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A55" s="18" t="s">
         <v>77</v>
       </c>
@@ -20120,7 +20398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A56" s="18" t="s">
         <v>78</v>
       </c>
@@ -20128,7 +20406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A57" s="18" t="s">
         <v>53</v>
       </c>

</xml_diff>